<commit_message>
check the place cross backgroung and aproximately line
</commit_message>
<xml_diff>
--- a/Our_Labs/Lab_2/Opracowanie wyników pomiaru.xlsx
+++ b/Our_Labs/Lab_2/Opracowanie wyników pomiaru.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polslpl-my.sharepoint.com/personal/kp306682_student_polsl_pl/Documents/Studia/#Fizyka/My_Labs/Lab_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryzen\Desktop\Git_repos\Fizyka\Our_Labs\Lab_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{D8DEDA97-7E27-4BBD-B856-3A477BCB0FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C905D643-FB4C-44DD-B7B3-ACB23EE07EC7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C305AA4-9701-4ABE-A78A-4064A8B9BA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF9499B3-2041-4EAF-A3E1-B3B3A6C7F9D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -410,6 +410,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -420,21 +435,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1636,6 +1636,30 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-67FD-4A19-8A2E-A18D7F529D71}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:xVal>
             <c:numRef>
               <c:f>(Arkusz1!$E$3,Arkusz1!$E$26)</c:f>
@@ -3009,13 +3033,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>585108</xdr:colOff>
+      <xdr:colOff>530679</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>108858</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:colOff>50346</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>66989</xdr:rowOff>
     </xdr:to>
@@ -3040,6 +3064,84 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>517071</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>128076</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>449205</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>181654</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="pole tekstowe 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6207FF4-EC71-6F2B-74C4-CB4006520EE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18494828" y="11786676"/>
+          <a:ext cx="541734" cy="244078"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>x</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="-25000">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>max</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3622,8 +3724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA0D3CE8-817A-4440-892E-9F3E81450C06}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K45" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K2"/>
+    <sheetView tabSelected="1" topLeftCell="L42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AD64" sqref="AD64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3656,16 +3758,16 @@
       <c r="H1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="15" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3680,16 +3782,16 @@
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="15"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="4">
@@ -3723,8 +3825,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
       <c r="E4" s="4">
         <v>0.03</v>
       </c>
@@ -4362,16 +4464,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>